<commit_message>
exclusion to white milk in ccanz
</commit_message>
<xml_diff>
--- a/Projects/CCANZ/Data/template.xlsx
+++ b/Projects/CCANZ/Data/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Exclude" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="18">
   <si>
     <t xml:space="preserve">KPI</t>
   </si>
@@ -53,7 +53,7 @@
     <t xml:space="preserve">category</t>
   </si>
   <si>
-    <t xml:space="preserve">FLAVOURED MILK,07- JUICE</t>
+    <t xml:space="preserve">Flavoured Milk,Juice</t>
   </si>
   <si>
     <t xml:space="preserve">size</t>
@@ -62,19 +62,13 @@
     <t xml:space="preserve">2,4,2.25,2.4,10,3</t>
   </si>
   <si>
-    <t xml:space="preserve">WHITE MILK,Irrelevant,General</t>
+    <t xml:space="preserve">Irrelevant,General,White milk</t>
   </si>
   <si>
     <t xml:space="preserve">Share of Shelf by Linear</t>
   </si>
   <si>
-    <t xml:space="preserve">FLAVOURED MILK, 07- JUICE</t>
-  </si>
-  <si>
     <t xml:space="preserve">Denominator</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FLAVOURED MILK,07- JUICE</t>
   </si>
   <si>
     <t xml:space="preserve">brand</t>
@@ -90,7 +84,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -138,6 +132,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -219,7 +219,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -245,6 +245,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -328,16 +332,16 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -394,7 +398,7 @@
       <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="6"/>
@@ -412,7 +416,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6" t="s">
@@ -432,7 +436,7 @@
       <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="6"/>
@@ -444,12 +448,12 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="6"/>
@@ -461,7 +465,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>9</v>
@@ -482,12 +486,12 @@
         <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="6"/>
@@ -499,13 +503,13 @@
         <v>14</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6" t="s">
@@ -533,18 +537,18 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.6071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.5255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -575,10 +579,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -588,13 +592,13 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -607,10 +611,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -620,13 +624,13 @@
         <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>

</xml_diff>